<commit_message>
Auto-push with fireball accuracy report [2025-04-12 08:40 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -528,13 +528,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>83.3</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="6">
@@ -666,16 +666,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
         <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>62.5</v>
+        <v>55.6</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-12 08:44 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
         <v>59</v>
       </c>
       <c r="D2" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" t="n">
-        <v>95.2</v>
+        <v>93.7</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>61</v>
       </c>
       <c r="D3" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" t="n">
-        <v>92.40000000000001</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="4">
@@ -506,16 +506,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>14</v>
       </c>
       <c r="D4" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
-        <v>77.8</v>
+        <v>73.7</v>
       </c>
     </row>
     <row r="5">
@@ -612,13 +612,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" t="n">
-        <v>93.7</v>
+        <v>93.8</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" t="n">
         <v>58</v>
       </c>
       <c r="E3" t="n">
-        <v>93.09999999999999</v>
+        <v>94.8</v>
       </c>
     </row>
     <row r="4">
@@ -666,16 +666,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
         <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>55.6</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-12 08:49 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>59</v>
       </c>
       <c r="D2" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="n">
-        <v>93.7</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
         <v>61</v>
       </c>
       <c r="D3" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E3" t="n">
-        <v>95.3</v>
+        <v>93.8</v>
       </c>
     </row>
     <row r="4">
@@ -631,13 +631,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" t="n">
-        <v>94.8</v>
+        <v>94.7</v>
       </c>
     </row>
     <row r="4">
@@ -669,13 +669,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>62.5</v>
+        <v>66.7</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-13 03:31 AM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D2" t="n">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E2" t="n">
-        <v>95.2</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D3" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E3" t="n">
-        <v>93.8</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4">
@@ -506,16 +506,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" t="n">
-        <v>73.7</v>
+        <v>81.2</v>
       </c>
     </row>
     <row r="5">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>85.7</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
@@ -544,16 +544,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>57.1</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -612,13 +612,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D2" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" t="n">
-        <v>93.8</v>
+        <v>93.90000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -631,13 +631,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" t="n">
-        <v>94.7</v>
+        <v>94.8</v>
       </c>
     </row>
     <row r="4">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D4" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" t="n">
-        <v>69.2</v>
+        <v>91.7</v>
       </c>
     </row>
     <row r="5">
@@ -669,13 +669,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" t="n">
-        <v>66.7</v>
+        <v>72.7</v>
       </c>
     </row>
     <row r="6">
@@ -685,16 +685,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>25</v>
+        <v>33.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-13 01:53 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -471,13 +471,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D2" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E2" t="n">
-        <v>97.2</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D3" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E3" t="n">
-        <v>95</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="4">
@@ -509,13 +509,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>81.2</v>
+        <v>82.40000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -612,13 +612,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D2" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E2" t="n">
-        <v>93.90000000000001</v>
+        <v>94.09999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>55</v>
       </c>
       <c r="D3" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E3" t="n">
-        <v>94.8</v>
+        <v>90.2</v>
       </c>
     </row>
     <row r="4">
@@ -669,13 +669,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>72.7</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-13 03:59 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" t="n">
         <v>74</v>
       </c>
       <c r="E2" t="n">
-        <v>97.3</v>
+        <v>95.90000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D3" t="n">
         <v>62</v>
       </c>
       <c r="E3" t="n">
-        <v>93.5</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="4">
@@ -509,13 +509,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="n">
-        <v>82.40000000000001</v>
+        <v>81.2</v>
       </c>
     </row>
     <row r="5">
@@ -528,13 +528,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">
@@ -547,13 +547,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>20</v>
+        <v>33.3</v>
       </c>
     </row>
   </sheetData>
@@ -609,16 +609,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="n">
-        <v>94.09999999999999</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" t="n">
-        <v>90.2</v>
+        <v>94.90000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" t="n">
-        <v>91.7</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="5">
@@ -685,13 +685,13 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
         <v>2</v>
       </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6" t="n">
         <v>33.3</v>

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-13 07:55 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E2" t="n">
-        <v>95.90000000000001</v>
+        <v>94.7</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
         <v>59</v>
       </c>
       <c r="D3" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E3" t="n">
-        <v>95.2</v>
+        <v>93.7</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
         <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>75</v>
+        <v>69.2</v>
       </c>
     </row>
     <row r="6">
@@ -612,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D2" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E2" t="n">
-        <v>92.5</v>
+        <v>92.8</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="n">
         <v>59</v>
       </c>
       <c r="E3" t="n">
-        <v>94.90000000000001</v>
+        <v>93.2</v>
       </c>
     </row>
     <row r="4">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>88.5</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="5">
@@ -666,16 +666,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>75</v>
+        <v>66.7</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-14 04:03 AM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D2" t="n">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E2" t="n">
-        <v>94.7</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>59</v>
       </c>
       <c r="D3" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" t="n">
-        <v>93.7</v>
+        <v>96.7</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>69.2</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="6">
@@ -547,13 +547,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>33.3</v>
+        <v>42.9</v>
       </c>
     </row>
   </sheetData>
@@ -609,16 +609,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D2" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E2" t="n">
-        <v>92.8</v>
+        <v>94.40000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D3" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E3" t="n">
-        <v>93.2</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E4" t="n">
-        <v>85.7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
@@ -666,16 +666,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
         <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="n">
-        <v>66.7</v>
+        <v>72.7</v>
       </c>
     </row>
     <row r="6">
@@ -685,16 +685,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>33.3</v>
+        <v>66.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-15 04:18 AM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -471,13 +471,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D2" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E2" t="n">
-        <v>96.3</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>59</v>
       </c>
       <c r="D3" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E3" t="n">
-        <v>96.7</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="4">
@@ -509,13 +509,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>81.2</v>
+        <v>82.40000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>62.5</v>
+        <v>77.8</v>
       </c>
     </row>
     <row r="6">
@@ -547,13 +547,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>42.9</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -609,16 +609,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D2" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E2" t="n">
-        <v>94.40000000000001</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D3" t="n">
         <v>66</v>
       </c>
       <c r="E3" t="n">
-        <v>97</v>
+        <v>92.40000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" t="n">
-        <v>87</v>
+        <v>95.8</v>
       </c>
     </row>
     <row r="5">
@@ -685,16 +685,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>66.7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-15 06:58 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -471,13 +471,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E2" t="n">
-        <v>96.5</v>
+        <v>96.59999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -490,10 +490,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D3" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E3" t="n">
         <v>95.2</v>
@@ -506,16 +506,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
-        <v>82.40000000000001</v>
+        <v>78.90000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -612,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D2" t="n">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E2" t="n">
-        <v>93.5</v>
+        <v>93.8</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>61</v>
       </c>
       <c r="D3" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E3" t="n">
-        <v>92.40000000000001</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-16 03:22 AM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D2" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E2" t="n">
-        <v>96.59999999999999</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D3" t="n">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E3" t="n">
-        <v>95.2</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="4">
@@ -509,13 +509,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E4" t="n">
-        <v>78.90000000000001</v>
+        <v>69.2</v>
       </c>
     </row>
     <row r="5">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>77.8</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="6">
@@ -544,16 +544,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>71.40000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -609,16 +609,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D2" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" t="n">
-        <v>93.8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D3" t="n">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E3" t="n">
-        <v>91</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="4">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D4" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" t="n">
-        <v>95.8</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="5">
@@ -666,16 +666,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E5" t="n">
-        <v>72.7</v>
+        <v>72.2</v>
       </c>
     </row>
     <row r="6">
@@ -685,16 +685,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-16 04:55 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -471,13 +471,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E2" t="n">
-        <v>94.5</v>
+        <v>94.59999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>66</v>
       </c>
       <c r="D3" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E3" t="n">
-        <v>94.3</v>
+        <v>91.7</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
         <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>61.5</v>
+        <v>57.1</v>
       </c>
     </row>
     <row r="6">
@@ -544,16 +544,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>71.40000000000001</v>
+        <v>62.5</v>
       </c>
     </row>
   </sheetData>
@@ -609,16 +609,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
         <v>71</v>
       </c>
       <c r="D2" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" t="n">
-        <v>91</v>
+        <v>89.90000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>71</v>
       </c>
       <c r="D3" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E3" t="n">
-        <v>97.3</v>
+        <v>95.90000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" t="n">
-        <v>76.2</v>
+        <v>73.90000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -688,13 +688,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-17 03:56 AM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" t="n">
-        <v>94.59999999999999</v>
+        <v>93.59999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E3" t="n">
-        <v>91.7</v>
+        <v>87.2</v>
       </c>
     </row>
     <row r="4">
@@ -509,13 +509,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
-        <v>69.2</v>
+        <v>78.90000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>57.1</v>
+        <v>77.8</v>
       </c>
     </row>
     <row r="6">
@@ -609,16 +609,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D2" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E2" t="n">
-        <v>89.90000000000001</v>
+        <v>93.90000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D3" t="n">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E3" t="n">
-        <v>95.90000000000001</v>
+        <v>90.2</v>
       </c>
     </row>
     <row r="4">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" t="n">
-        <v>73.90000000000001</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="5">
@@ -666,16 +666,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>72.2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
@@ -685,16 +685,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-push with fireball accuracy report [2025-04-17 03:35 PM]
</commit_message>
<xml_diff>
--- a/fireball_accuracy_report.xlsx
+++ b/fireball_accuracy_report.xlsx
@@ -490,13 +490,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D3" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E3" t="n">
-        <v>87.2</v>
+        <v>87.3</v>
       </c>
     </row>
     <row r="4">
@@ -506,16 +506,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="n">
-        <v>78.90000000000001</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
         <v>21</v>
       </c>
       <c r="D4" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" t="n">
-        <v>87.5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
@@ -688,13 +688,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>